<commit_message>
Tidy up of switch to holder class
</commit_message>
<xml_diff>
--- a/threading data.xlsx
+++ b/threading data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ostandage/UEA OneDrive/OneDrive - University of East Anglia/Year 3/6013Y - Project/tsml/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ostandage/GitRepos/tsml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{3B44101F-9B24-9747-BC99-523905ECEEBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00B0BEB7-CB5C-6144-81C4-DED7E7FB57B6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84740801-9404-D14B-92A2-9EB24CFDA902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="1620" windowWidth="38400" windowHeight="22760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="G4 (Iteration 1)" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>Classifier</t>
   </si>
@@ -72,6 +74,12 @@
   </si>
   <si>
     <t>Overhead of maintaing the SortedMap</t>
+  </si>
+  <si>
+    <t>4 (class)</t>
+  </si>
+  <si>
+    <t>Vars (4)</t>
   </si>
 </sst>
 </file>
@@ -558,9 +566,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -622,7 +631,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1044,7 +1053,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1466,7 +1475,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1559,9 +1568,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Pi4 (TreeMap)'!$A$2:$A$5</c:f>
+              <c:f>'Pi4 (TreeMap)'!$A$2:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Control (1)</c:v>
                 </c:pt>
@@ -1574,15 +1583,18 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Vars (4)</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pi4 (TreeMap)'!$E$2:$E$5</c:f>
+              <c:f>'Pi4 (TreeMap)'!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>62753960.163999997</c:v>
                 </c:pt>
@@ -1594,6 +1606,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>27441388.873</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>26822213.548999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3947,7 +3962,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A7" sqref="A7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4062,7 +4077,7 @@
         <v>2428275539</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H5" si="0">100*(1-(E4/$E$2))</f>
+        <f t="shared" ref="H4:H7" si="0">100*(1-(E4/$E$2))</f>
         <v>39.014495664289427</v>
       </c>
     </row>
@@ -4094,9 +4109,31 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2828352.2450000001</v>
+      </c>
+      <c r="F6">
+        <v>10860872620</v>
+      </c>
+      <c r="G6">
+        <v>1568099091</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>64.460860009899818</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4271,7 +4308,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4359,7 +4396,7 @@
         <v>18426871459</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H5" si="0">100*(1-(E3/$E$2))</f>
+        <f t="shared" ref="H3:H6" si="0">100*(1-(E3/$E$2))</f>
         <v>33.016629160697953</v>
       </c>
     </row>
@@ -4418,9 +4455,31 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>26822213.548999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>102997300027</v>
+      </c>
+      <c r="G6" s="1">
+        <v>12038206017</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>57.258134022293831</v>
+      </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">

</xml_diff>